<commit_message>
add XGB, change MLP layer number
</commit_message>
<xml_diff>
--- a/2/code/results-summary.xlsx
+++ b/2/code/results-summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">data set\model</t>
   </si>
@@ -38,6 +38,15 @@
   </si>
   <si>
     <t xml:space="preserve">Random forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP(10,256)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLP(30,1024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xgboost</t>
   </si>
   <si>
     <t xml:space="preserve">20 news group</t>
@@ -58,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,6 +89,7 @@
       <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,19 +220,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -243,10 +256,19 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.776</v>
@@ -262,11 +284,20 @@
       </c>
       <c r="F2" s="0" t="n">
         <v>0.688</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.7058</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0.7408</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0.6164</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.883</v>
@@ -282,6 +313,15 @@
       </c>
       <c r="F3" s="0" t="n">
         <v>0.8367</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.8757</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0.8801</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0.7398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>